<commit_message>
Quick fix of magnitude for PB2003
</commit_message>
<xml_diff>
--- a/budget/data/JSF 0603800.xlsx
+++ b/budget/data/JSF 0603800.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Greg\Repositories\Engines\budget\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AA90A3-899B-45BD-8628-48196FD60152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F74D63-A3F3-4ABB-9D25-F7A928ECAB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33300" yWindow="1485" windowWidth="19500" windowHeight="13485" xr2:uid="{0A31612C-3C2D-45DF-B35A-9F610161C2CC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A31612C-3C2D-45DF-B35A-9F610161C2CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="64">
   <si>
     <t>Contract Method &amp; Type</t>
   </si>
@@ -225,14 +225,25 @@
   </si>
   <si>
     <t>Oct 99-Sep 00</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -260,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -270,6 +281,8 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C332E7-8D05-4EDA-93F1-A9AA89CD670B}">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,11 +610,11 @@
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" x14ac:dyDescent="0.25">
@@ -1153,26 +1166,29 @@
       <c r="G17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="2">
-        <v>10100</v>
-      </c>
-      <c r="J17" s="2">
-        <v>10100</v>
-      </c>
-      <c r="K17" s="2">
-        <v>10100</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2">
-        <v>10100</v>
+      <c r="I17" s="8">
+        <v>10.1</v>
+      </c>
+      <c r="J17" s="8">
+        <v>10.1</v>
+      </c>
+      <c r="K17" s="8">
+        <v>10.1</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0</v>
+      </c>
+      <c r="P17" s="8">
+        <v>10.1</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1200,126 +1216,112 @@
       <c r="H18" s="4">
         <v>36161</v>
       </c>
-      <c r="I18" s="2">
-        <v>1500</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1500</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1500</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="I18" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0</v>
+      </c>
+      <c r="N18" s="8">
+        <v>0</v>
+      </c>
+      <c r="O18" s="8">
+        <v>0</v>
+      </c>
+      <c r="P18" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2">
+        <f>SUBTOTAL(9,K2:K18)*1000</f>
+        <v>1142058.0000000002</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" ref="L19:P19" si="0">SUBTOTAL(9,L2:L18)*1000</f>
+        <v>314557</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="0"/>
+        <v>1456615.0000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>29</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2002</v>
-      </c>
-      <c r="B21">
-        <v>603800</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="2">
-        <v>954076</v>
-      </c>
-      <c r="J21" s="2">
-        <v>954076</v>
-      </c>
-      <c r="K21" s="2">
-        <v>750071</v>
-      </c>
-      <c r="L21" s="2">
-        <v>87019</v>
-      </c>
-      <c r="M21" s="2">
-        <v>127694</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" s="2">
-        <v>964784</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1336,22 +1338,40 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="5">
-        <v>44652</v>
+      <c r="H22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="2">
+        <v>954076</v>
+      </c>
+      <c r="J22" s="2">
+        <v>954076</v>
+      </c>
+      <c r="K22" s="2">
+        <v>750071</v>
+      </c>
+      <c r="L22" s="2">
+        <v>87019</v>
       </c>
       <c r="M22" s="2">
-        <v>85334</v>
+        <v>127694</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
       </c>
       <c r="P22" s="2">
-        <v>85334</v>
+        <v>964784</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1368,40 +1388,22 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
       </c>
-      <c r="H23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="2">
-        <v>7000</v>
-      </c>
-      <c r="J23" s="2">
-        <v>7000</v>
-      </c>
-      <c r="K23" s="2">
-        <v>7000</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
+      <c r="H23" s="5">
+        <v>44652</v>
       </c>
       <c r="M23" s="2">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
+        <v>85334</v>
       </c>
       <c r="P23" s="2">
-        <v>7000</v>
+        <v>85334</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1426,20 +1428,23 @@
       <c r="G24" t="s">
         <v>11</v>
       </c>
+      <c r="H24" t="s">
+        <v>45</v>
+      </c>
       <c r="I24" s="2">
-        <v>183728</v>
+        <v>7000</v>
       </c>
       <c r="J24" s="2">
-        <v>183728</v>
+        <v>7000</v>
       </c>
       <c r="K24" s="2">
-        <v>103397</v>
-      </c>
-      <c r="L24" s="2">
-        <v>34710</v>
+        <v>7000</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
       </c>
       <c r="M24" s="2">
-        <v>45620</v>
+        <v>0</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -1448,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="2">
-        <v>183727</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1465,28 +1470,28 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I25" s="2">
-        <v>5448</v>
+        <v>183728</v>
       </c>
       <c r="J25" s="2">
-        <v>5448</v>
+        <v>183728</v>
       </c>
       <c r="K25" s="2">
-        <v>5448</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
+        <v>103397</v>
+      </c>
+      <c r="L25" s="2">
+        <v>34710</v>
+      </c>
+      <c r="M25" s="2">
+        <v>45620</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -1495,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="2">
-        <v>5448</v>
+        <v>183727</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1515,19 +1520,19 @@
         <v>19</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="I26" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
       <c r="J26" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
       <c r="K26" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1542,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1562,19 +1567,19 @@
         <v>19</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
       <c r="J27" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
       <c r="K27" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -1589,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1609,19 +1614,19 @@
         <v>19</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
       </c>
       <c r="I28" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="J28" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="K28" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1636,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1656,22 +1661,19 @@
         <v>19</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="4">
-        <v>36161</v>
-      </c>
       <c r="I29" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
       <c r="J29" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
       <c r="K29" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -1686,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -1706,19 +1708,22 @@
         <v>19</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
+      <c r="H30" s="4">
+        <v>36161</v>
+      </c>
       <c r="I30" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
       <c r="J30" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
       <c r="K30" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1733,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -1756,19 +1761,16 @@
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="4">
-        <v>36130</v>
+        <v>11</v>
       </c>
       <c r="I31" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
       <c r="J31" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
       <c r="K31" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -1783,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1803,22 +1805,22 @@
         <v>19</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H32" s="4">
-        <v>36342</v>
+        <v>36130</v>
       </c>
       <c r="I32" s="2">
-        <v>2800</v>
+        <v>8200</v>
       </c>
       <c r="J32" s="2">
-        <v>2800</v>
+        <v>8200</v>
       </c>
       <c r="K32" s="2">
-        <v>2800</v>
+        <v>8200</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -1833,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="2">
-        <v>2800</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -1856,25 +1858,25 @@
         <v>23</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="H33" s="4">
+        <v>36342</v>
       </c>
       <c r="I33" s="2">
-        <v>14845</v>
+        <v>2800</v>
       </c>
       <c r="J33" s="2">
-        <v>14845</v>
+        <v>2800</v>
       </c>
       <c r="K33" s="2">
-        <v>14699</v>
+        <v>2800</v>
       </c>
       <c r="L33">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -1883,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="2">
-        <v>14845</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -1906,25 +1908,25 @@
         <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="I34" s="2">
-        <v>51011</v>
+        <v>14845</v>
       </c>
       <c r="J34" s="2">
-        <v>51011</v>
+        <v>14845</v>
       </c>
       <c r="K34" s="2">
-        <v>39873</v>
-      </c>
-      <c r="L34" s="2">
-        <v>8020</v>
-      </c>
-      <c r="M34" s="2">
-        <v>2990</v>
+        <v>14699</v>
+      </c>
+      <c r="L34">
+        <v>96</v>
+      </c>
+      <c r="M34">
+        <v>50</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -1933,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="2">
-        <v>50883</v>
+        <v>14845</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -1950,28 +1952,31 @@
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G35" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="H35" t="s">
+        <v>49</v>
       </c>
       <c r="I35" s="2">
-        <v>10100</v>
+        <v>51011</v>
       </c>
       <c r="J35" s="2">
-        <v>10100</v>
+        <v>51011</v>
       </c>
       <c r="K35" s="2">
-        <v>10100</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
+        <v>39873</v>
+      </c>
+      <c r="L35" s="2">
+        <v>8020</v>
+      </c>
+      <c r="M35" s="2">
+        <v>2990</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -1980,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="P35" s="2">
-        <v>10100</v>
+        <v>50883</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2000,142 +2005,170 @@
         <v>52</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G36" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="4">
+      <c r="I36" s="2">
+        <v>10100</v>
+      </c>
+      <c r="J36" s="2">
+        <v>10100</v>
+      </c>
+      <c r="K36" s="2">
+        <v>10100</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2002</v>
+      </c>
+      <c r="B37">
+        <v>603800</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="4">
         <v>36161</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I37" s="2">
         <v>1500</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J37" s="2">
         <v>1500</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K37" s="2">
         <v>1500</v>
       </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36" s="2">
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
         <v>1500</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F37" s="3"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F38" s="3"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="2">
+        <f>SUBTOTAL(9,I21:I37)</f>
+        <v>1307806</v>
+      </c>
+      <c r="J38" s="2">
+        <f>SUBTOTAL(9,J21:J37)</f>
+        <v>1307806</v>
+      </c>
+      <c r="K38" s="2">
+        <f>SUBTOTAL(9,K21:K37)</f>
+        <v>1012186</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" ref="L38:P38" si="1">SUBTOTAL(9,L21:L37)</f>
+        <v>129845</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="1"/>
+        <v>261688</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="1"/>
+        <v>1403719</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>28</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>29</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2001</v>
-      </c>
-      <c r="B39">
-        <v>603800</v>
-      </c>
-      <c r="C39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
-        <v>49</v>
-      </c>
-      <c r="I39" s="2">
-        <v>914471</v>
-      </c>
-      <c r="J39" s="2">
-        <v>914471</v>
-      </c>
-      <c r="K39" s="2">
-        <v>537405</v>
-      </c>
-      <c r="L39" s="2">
-        <v>212666</v>
-      </c>
-      <c r="M39" s="2">
-        <v>84200</v>
-      </c>
-      <c r="N39" s="2">
-        <v>80200</v>
-      </c>
-      <c r="P39" s="2">
-        <v>914471</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -2152,28 +2185,37 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I40" s="2">
-        <v>7000</v>
+        <v>914471</v>
       </c>
       <c r="J40" s="2">
-        <v>7000</v>
+        <v>914471</v>
       </c>
       <c r="K40" s="2">
-        <v>7000</v>
+        <v>537405</v>
+      </c>
+      <c r="L40" s="2">
+        <v>212666</v>
+      </c>
+      <c r="M40" s="2">
+        <v>84200</v>
+      </c>
+      <c r="N40" s="2">
+        <v>80200</v>
       </c>
       <c r="P40" s="2">
-        <v>7000</v>
+        <v>914471</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -2198,26 +2240,20 @@
       <c r="G41" t="s">
         <v>11</v>
       </c>
+      <c r="H41" t="s">
+        <v>45</v>
+      </c>
       <c r="I41" s="2">
-        <v>222137</v>
+        <v>7000</v>
       </c>
       <c r="J41" s="2">
-        <v>222137</v>
+        <v>7000</v>
       </c>
       <c r="K41" s="2">
-        <v>61794</v>
-      </c>
-      <c r="L41" s="2">
-        <v>40153</v>
-      </c>
-      <c r="M41" s="2">
-        <v>26190</v>
-      </c>
-      <c r="N41" s="2">
-        <v>94000</v>
+        <v>7000</v>
       </c>
       <c r="P41" s="2">
-        <v>222137</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -2234,25 +2270,34 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G42" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I42" s="2">
-        <v>5448</v>
+        <v>222137</v>
       </c>
       <c r="J42" s="2">
-        <v>5448</v>
+        <v>222137</v>
       </c>
       <c r="K42" s="2">
-        <v>5448</v>
+        <v>61794</v>
+      </c>
+      <c r="L42" s="2">
+        <v>40153</v>
+      </c>
+      <c r="M42" s="2">
+        <v>26190</v>
+      </c>
+      <c r="N42" s="2">
+        <v>94000</v>
       </c>
       <c r="P42" s="2">
-        <v>5448</v>
+        <v>222137</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -2272,22 +2317,22 @@
         <v>19</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="I43" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
       <c r="J43" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
       <c r="K43" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
       <c r="P43" s="2">
-        <v>5681</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -2307,22 +2352,22 @@
         <v>19</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G44" t="s">
         <v>11</v>
       </c>
       <c r="I44" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
       <c r="J44" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
       <c r="K44" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
       <c r="P44" s="2">
-        <v>30000</v>
+        <v>5681</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -2342,22 +2387,22 @@
         <v>19</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G45" t="s">
         <v>11</v>
       </c>
       <c r="I45" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="J45" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="K45" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
       <c r="P45" s="2">
-        <v>3000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -2377,28 +2422,22 @@
         <v>19</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G46" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="4">
-        <v>36161</v>
-      </c>
       <c r="I46" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
       <c r="J46" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
       <c r="K46" s="2">
-        <v>22988</v>
-      </c>
-      <c r="L46" s="2">
-        <v>3789</v>
+        <v>3000</v>
       </c>
       <c r="P46" s="2">
-        <v>26777</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -2418,22 +2457,28 @@
         <v>19</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G47" t="s">
         <v>11</v>
       </c>
+      <c r="H47" s="4">
+        <v>36161</v>
+      </c>
       <c r="I47" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
       <c r="J47" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
       <c r="K47" s="2">
-        <v>3640</v>
+        <v>22988</v>
+      </c>
+      <c r="L47" s="2">
+        <v>3789</v>
       </c>
       <c r="P47" s="2">
-        <v>3640</v>
+        <v>26777</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -2456,25 +2501,19 @@
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H48" s="4">
-        <v>36130</v>
+        <v>11</v>
       </c>
       <c r="I48" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
       <c r="J48" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
       <c r="K48" s="2">
-        <v>7000</v>
-      </c>
-      <c r="L48" s="2">
-        <v>1200</v>
+        <v>3640</v>
       </c>
       <c r="P48" s="2">
-        <v>8200</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -2494,28 +2533,28 @@
         <v>19</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H49" s="4">
-        <v>36342</v>
+        <v>36130</v>
       </c>
       <c r="I49" s="2">
-        <v>2800</v>
+        <v>8200</v>
       </c>
       <c r="J49" s="2">
-        <v>2800</v>
-      </c>
-      <c r="K49">
-        <v>700</v>
+        <v>8200</v>
+      </c>
+      <c r="K49" s="2">
+        <v>7000</v>
       </c>
       <c r="L49" s="2">
-        <v>2100</v>
+        <v>1200</v>
       </c>
       <c r="P49" s="2">
-        <v>2800</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -2538,31 +2577,25 @@
         <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="H50" s="4">
+        <v>36342</v>
       </c>
       <c r="I50" s="2">
-        <v>14979</v>
+        <v>2800</v>
       </c>
       <c r="J50" s="2">
-        <v>14979</v>
-      </c>
-      <c r="K50" s="2">
-        <v>12895</v>
+        <v>2800</v>
+      </c>
+      <c r="K50">
+        <v>700</v>
       </c>
       <c r="L50" s="2">
-        <v>1804</v>
-      </c>
-      <c r="M50">
-        <v>48</v>
-      </c>
-      <c r="N50">
-        <v>50</v>
+        <v>2100</v>
       </c>
       <c r="P50" s="2">
-        <v>14797</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -2585,31 +2618,31 @@
         <v>23</v>
       </c>
       <c r="G51" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="I51" s="2">
-        <v>50020</v>
+        <v>14979</v>
       </c>
       <c r="J51" s="2">
-        <v>50020</v>
+        <v>14979</v>
       </c>
       <c r="K51" s="2">
-        <v>24484</v>
+        <v>12895</v>
       </c>
       <c r="L51" s="2">
-        <v>15389</v>
-      </c>
-      <c r="M51" s="2">
-        <v>7197</v>
-      </c>
-      <c r="N51" s="2">
-        <v>2950</v>
+        <v>1804</v>
+      </c>
+      <c r="M51">
+        <v>48</v>
+      </c>
+      <c r="N51">
+        <v>50</v>
       </c>
       <c r="P51" s="2">
-        <v>50020</v>
+        <v>14797</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -2626,25 +2659,37 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G52" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="H52" t="s">
+        <v>49</v>
       </c>
       <c r="I52" s="2">
-        <v>10100</v>
+        <v>50020</v>
       </c>
       <c r="J52" s="2">
-        <v>10100</v>
+        <v>50020</v>
       </c>
       <c r="K52" s="2">
-        <v>10100</v>
+        <v>24484</v>
+      </c>
+      <c r="L52" s="2">
+        <v>15389</v>
+      </c>
+      <c r="M52" s="2">
+        <v>7197</v>
+      </c>
+      <c r="N52" s="2">
+        <v>2950</v>
       </c>
       <c r="P52" s="2">
-        <v>10100</v>
+        <v>50020</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -2664,181 +2709,157 @@
         <v>53</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G53" t="s">
         <v>20</v>
       </c>
-      <c r="H53" s="4">
+      <c r="I53" s="2">
+        <v>10100</v>
+      </c>
+      <c r="J53" s="2">
+        <v>10100</v>
+      </c>
+      <c r="K53" s="2">
+        <v>10100</v>
+      </c>
+      <c r="P53" s="2">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2001</v>
+      </c>
+      <c r="B54">
+        <v>603800</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G54" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="4">
         <v>36161</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I54" s="2">
         <v>1500</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J54" s="2">
         <v>1500</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L54" s="2">
         <v>1500</v>
       </c>
-      <c r="P53" s="2">
+      <c r="P54" s="2">
         <v>1500</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F54" s="3"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="P54" s="2"/>
-    </row>
-    <row r="55" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F55" s="3"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="2">
+        <f>SUBTOTAL(9,I38:I54)</f>
+        <v>1305753</v>
+      </c>
+      <c r="J55" s="2">
+        <f>SUBTOTAL(9,J38:J54)</f>
+        <v>1305753</v>
+      </c>
+      <c r="K55" s="2">
+        <f>SUBTOTAL(9,K38:K54)</f>
+        <v>732135</v>
+      </c>
+      <c r="L55" s="2">
+        <f t="shared" ref="L55" si="2">SUBTOTAL(9,L38:L54)</f>
+        <v>278601</v>
+      </c>
+      <c r="M55" s="2">
+        <f t="shared" ref="M55" si="3">SUBTOTAL(9,M38:M54)</f>
+        <v>117635</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" ref="N55" si="4">SUBTOTAL(9,N38:N54)</f>
+        <v>177200</v>
+      </c>
+      <c r="O55" s="2">
+        <f t="shared" ref="O55" si="5">SUBTOTAL(9,O38:O54)</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="2">
+        <f t="shared" ref="P55" si="6">SUBTOTAL(9,P38:P54)</f>
+        <v>1305571</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F56" s="3"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="P56" s="2"/>
+    </row>
+    <row r="57" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>41</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>28</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>29</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="L57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="M57" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N55" s="1" t="s">
+      <c r="N57" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O55" s="1" t="s">
+      <c r="O57" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P55" s="1" t="s">
+      <c r="P57" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q55" s="1" t="s">
+      <c r="Q57" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>2000</v>
-      </c>
-      <c r="B56">
-        <v>603800</v>
-      </c>
-      <c r="C56" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" s="4">
-        <v>35370</v>
-      </c>
-      <c r="I56" s="2">
-        <v>751148</v>
-      </c>
-      <c r="J56" s="2">
-        <v>751148</v>
-      </c>
-      <c r="K56" s="2">
-        <v>216936</v>
-      </c>
-      <c r="L56" s="2">
-        <v>285230</v>
-      </c>
-      <c r="M56" s="2">
-        <v>188808</v>
-      </c>
-      <c r="N56" s="2">
-        <v>59974</v>
-      </c>
-      <c r="O56">
-        <v>200</v>
-      </c>
-      <c r="Q56" s="2">
-        <v>751148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>2000</v>
-      </c>
-      <c r="B57">
-        <v>603800</v>
-      </c>
-      <c r="C57" t="s">
-        <v>30</v>
-      </c>
-      <c r="D57">
-        <v>4</v>
-      </c>
-      <c r="E57" t="s">
-        <v>60</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="2">
-        <v>77070</v>
-      </c>
-      <c r="J57" s="2">
-        <v>77070</v>
-      </c>
-      <c r="K57" s="2">
-        <v>14683</v>
-      </c>
-      <c r="L57" s="2">
-        <v>20369</v>
-      </c>
-      <c r="M57" s="2">
-        <v>25792</v>
-      </c>
-      <c r="N57" s="2">
-        <v>16226</v>
-      </c>
-      <c r="Q57" s="2">
-        <v>77070</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -2855,10 +2876,10 @@
         <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G58" t="s">
         <v>11</v>
@@ -2867,14 +2888,28 @@
         <v>35370</v>
       </c>
       <c r="I58" s="2">
-        <v>7000</v>
+        <v>751148</v>
       </c>
       <c r="J58" s="2">
-        <v>7000</v>
-      </c>
-      <c r="P58" s="2"/>
+        <v>751148</v>
+      </c>
+      <c r="K58" s="2">
+        <v>216936</v>
+      </c>
+      <c r="L58" s="2">
+        <v>285230</v>
+      </c>
+      <c r="M58" s="2">
+        <v>188808</v>
+      </c>
+      <c r="N58" s="2">
+        <v>59974</v>
+      </c>
+      <c r="O58">
+        <v>200</v>
+      </c>
       <c r="Q58" s="2">
-        <v>7000</v>
+        <v>751148</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -2891,38 +2926,35 @@
         <v>4</v>
       </c>
       <c r="E59" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G59" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" s="4">
-        <v>35462</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H59" s="4"/>
       <c r="I59" s="2">
-        <v>118746</v>
+        <v>77070</v>
       </c>
       <c r="J59" s="2">
-        <v>118746</v>
+        <v>77070</v>
       </c>
       <c r="K59" s="2">
-        <v>25000</v>
+        <v>14683</v>
       </c>
       <c r="L59" s="2">
-        <v>34956</v>
+        <v>20369</v>
       </c>
       <c r="M59" s="2">
-        <v>25790</v>
+        <v>25792</v>
       </c>
       <c r="N59" s="2">
-        <v>33000</v>
-      </c>
-      <c r="P59" s="2"/>
+        <v>16226</v>
+      </c>
       <c r="Q59" s="2">
-        <v>118746</v>
+        <v>77070</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -2939,29 +2971,26 @@
         <v>4</v>
       </c>
       <c r="E60" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H60" s="4">
-        <v>34669</v>
+        <v>35370</v>
       </c>
       <c r="I60" s="2">
-        <v>5448</v>
+        <v>7000</v>
       </c>
       <c r="J60" s="2">
-        <v>5448</v>
-      </c>
-      <c r="K60" s="2">
-        <v>5448</v>
+        <v>7000</v>
       </c>
       <c r="P60" s="2"/>
       <c r="Q60" s="2">
-        <v>5448</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -2978,29 +3007,38 @@
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G61" t="s">
         <v>11</v>
       </c>
       <c r="H61" s="4">
-        <v>34669</v>
+        <v>35462</v>
       </c>
       <c r="I61" s="2">
-        <v>5681</v>
+        <v>118746</v>
       </c>
       <c r="J61" s="2">
-        <v>5681</v>
+        <v>118746</v>
       </c>
       <c r="K61" s="2">
-        <v>5681</v>
+        <v>25000</v>
+      </c>
+      <c r="L61" s="2">
+        <v>34956</v>
+      </c>
+      <c r="M61" s="2">
+        <v>25790</v>
+      </c>
+      <c r="N61" s="2">
+        <v>33000</v>
       </c>
       <c r="P61" s="2"/>
       <c r="Q61" s="2">
-        <v>5681</v>
+        <v>118746</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -3023,23 +3061,23 @@
         <v>21</v>
       </c>
       <c r="G62" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H62" s="4">
-        <v>35004</v>
+        <v>34669</v>
       </c>
       <c r="I62" s="2">
-        <v>30000</v>
+        <v>5448</v>
       </c>
       <c r="J62" s="2">
-        <v>30000</v>
+        <v>5448</v>
       </c>
       <c r="K62" s="2">
-        <v>30000</v>
+        <v>5448</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" s="2">
-        <v>30000</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -3065,20 +3103,20 @@
         <v>11</v>
       </c>
       <c r="H63" s="4">
-        <v>35462</v>
+        <v>34669</v>
       </c>
       <c r="I63" s="2">
-        <v>3000</v>
+        <v>5681</v>
       </c>
       <c r="J63" s="2">
-        <v>3000</v>
+        <v>5681</v>
       </c>
       <c r="K63" s="2">
-        <v>3000</v>
+        <v>5681</v>
       </c>
       <c r="P63" s="2"/>
       <c r="Q63" s="2">
-        <v>3000</v>
+        <v>5681</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -3104,26 +3142,20 @@
         <v>11</v>
       </c>
       <c r="H64" s="4">
-        <v>35462</v>
+        <v>35004</v>
       </c>
       <c r="I64" s="2">
-        <v>26777</v>
+        <v>30000</v>
       </c>
       <c r="J64" s="2">
-        <v>26777</v>
+        <v>30000</v>
       </c>
       <c r="K64" s="2">
-        <v>10559</v>
-      </c>
-      <c r="L64" s="2">
-        <v>12429</v>
-      </c>
-      <c r="M64" s="2">
-        <v>3789</v>
+        <v>30000</v>
       </c>
       <c r="P64" s="2"/>
       <c r="Q64" s="2">
-        <v>26777</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -3143,26 +3175,26 @@
         <v>19</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G65" t="s">
         <v>11</v>
       </c>
       <c r="H65" s="4">
-        <v>35490</v>
+        <v>35462</v>
       </c>
       <c r="I65" s="2">
-        <v>3640</v>
+        <v>3000</v>
       </c>
       <c r="J65" s="2">
-        <v>3640</v>
+        <v>3000</v>
       </c>
       <c r="K65" s="2">
-        <v>3640</v>
+        <v>3000</v>
       </c>
       <c r="P65" s="2"/>
       <c r="Q65" s="2">
-        <v>3640</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -3182,32 +3214,32 @@
         <v>19</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G66" t="s">
-        <v>22</v>
-      </c>
-      <c r="H66" s="6">
-        <v>35765</v>
+        <v>11</v>
+      </c>
+      <c r="H66" s="4">
+        <v>35462</v>
       </c>
       <c r="I66" s="2">
-        <v>8200</v>
+        <v>26777</v>
       </c>
       <c r="J66" s="2">
-        <v>8200</v>
+        <v>26777</v>
       </c>
       <c r="K66" s="2">
-        <v>2400</v>
+        <v>10559</v>
       </c>
       <c r="L66" s="2">
-        <v>4600</v>
+        <v>12429</v>
       </c>
       <c r="M66" s="2">
-        <v>1200</v>
+        <v>3789</v>
       </c>
       <c r="P66" s="2"/>
       <c r="Q66" s="2">
-        <v>8200</v>
+        <v>26777</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -3227,26 +3259,26 @@
         <v>19</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G67" t="s">
-        <v>25</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>61</v>
+        <v>11</v>
+      </c>
+      <c r="H67" s="4">
+        <v>35490</v>
       </c>
       <c r="I67" s="2">
-        <v>700</v>
+        <v>3640</v>
       </c>
       <c r="J67" s="2">
-        <v>700</v>
-      </c>
-      <c r="L67">
-        <v>700</v>
+        <v>3640</v>
+      </c>
+      <c r="K67" s="2">
+        <v>3640</v>
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" s="2">
-        <v>700</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -3266,26 +3298,32 @@
         <v>19</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G68" t="s">
-        <v>24</v>
-      </c>
-      <c r="H68" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H68" s="6">
+        <v>35765</v>
       </c>
       <c r="I68" s="2">
-        <v>12895</v>
+        <v>8200</v>
       </c>
       <c r="J68" s="2">
-        <v>12895</v>
+        <v>8200</v>
       </c>
       <c r="K68" s="2">
-        <v>12895</v>
+        <v>2400</v>
+      </c>
+      <c r="L68" s="2">
+        <v>4600</v>
+      </c>
+      <c r="M68" s="2">
+        <v>1200</v>
       </c>
       <c r="P68" s="2"/>
       <c r="Q68" s="2">
-        <v>12895</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -3308,32 +3346,23 @@
         <v>23</v>
       </c>
       <c r="G69" t="s">
-        <v>26</v>
-      </c>
-      <c r="H69" t="s">
-        <v>62</v>
+        <v>25</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="I69" s="2">
-        <v>46132</v>
+        <v>700</v>
       </c>
       <c r="J69" s="2">
-        <v>46132</v>
-      </c>
-      <c r="K69" s="2">
-        <v>5897</v>
-      </c>
-      <c r="L69" s="2">
-        <v>18587</v>
-      </c>
-      <c r="M69" s="2">
-        <v>18048</v>
-      </c>
-      <c r="N69" s="2">
-        <v>3600</v>
+        <v>700</v>
+      </c>
+      <c r="L69">
+        <v>700</v>
       </c>
       <c r="P69" s="2"/>
       <c r="Q69" s="2">
-        <v>46132</v>
+        <v>700</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -3350,32 +3379,29 @@
         <v>4</v>
       </c>
       <c r="E70" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G70" t="s">
-        <v>20</v>
-      </c>
-      <c r="H70" s="4">
-        <v>35582</v>
+        <v>24</v>
+      </c>
+      <c r="H70" t="s">
+        <v>23</v>
       </c>
       <c r="I70" s="2">
-        <v>10100</v>
+        <v>12895</v>
       </c>
       <c r="J70" s="2">
-        <v>10100</v>
+        <v>12895</v>
       </c>
       <c r="K70" s="2">
-        <v>3920</v>
-      </c>
-      <c r="L70" s="2">
-        <v>6180</v>
+        <v>12895</v>
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" s="2">
-        <v>10100</v>
+        <v>12895</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -3392,213 +3418,208 @@
         <v>4</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="G71" t="s">
-        <v>20</v>
-      </c>
-      <c r="H71" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="H71" t="s">
+        <v>62</v>
+      </c>
       <c r="I71" s="2">
-        <v>1500</v>
+        <v>46132</v>
       </c>
       <c r="J71" s="2">
-        <v>1500</v>
-      </c>
-      <c r="L71" s="2"/>
+        <v>46132</v>
+      </c>
+      <c r="K71" s="2">
+        <v>5897</v>
+      </c>
+      <c r="L71" s="2">
+        <v>18587</v>
+      </c>
       <c r="M71" s="2">
-        <v>1500</v>
+        <v>18048</v>
+      </c>
+      <c r="N71" s="2">
+        <v>3600</v>
       </c>
       <c r="P71" s="2"/>
       <c r="Q71" s="2">
+        <v>46132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2000</v>
+      </c>
+      <c r="B72">
+        <v>603800</v>
+      </c>
+      <c r="C72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72">
+        <v>4</v>
+      </c>
+      <c r="E72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="4">
+        <v>35582</v>
+      </c>
+      <c r="I72" s="2">
+        <v>10100</v>
+      </c>
+      <c r="J72" s="2">
+        <v>10100</v>
+      </c>
+      <c r="K72" s="2">
+        <v>3920</v>
+      </c>
+      <c r="L72" s="2">
+        <v>6180</v>
+      </c>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2000</v>
+      </c>
+      <c r="B73">
+        <v>603800</v>
+      </c>
+      <c r="C73" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>53</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G73" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="4"/>
+      <c r="I73" s="2">
         <v>1500</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="J73" s="2">
+        <v>1500</v>
+      </c>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2">
+        <v>1500</v>
+      </c>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F74" s="3"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="2">
+        <f>SUBTOTAL(9,I57:I73)</f>
+        <v>1108037</v>
+      </c>
+      <c r="J74" s="2">
+        <f>SUBTOTAL(9,J57:J73)</f>
+        <v>1108037</v>
+      </c>
+      <c r="K74" s="2">
+        <f>SUBTOTAL(9,K57:K73)</f>
+        <v>340059</v>
+      </c>
+      <c r="L74" s="2">
+        <f t="shared" ref="L74" si="7">SUBTOTAL(9,L57:L73)</f>
+        <v>383051</v>
+      </c>
+      <c r="M74" s="2">
+        <f t="shared" ref="M74" si="8">SUBTOTAL(9,M57:M73)</f>
+        <v>264927</v>
+      </c>
+      <c r="N74" s="2">
+        <f t="shared" ref="N74" si="9">SUBTOTAL(9,N57:N73)</f>
+        <v>112800</v>
+      </c>
+      <c r="O74" s="2">
+        <f t="shared" ref="O74" si="10">SUBTOTAL(9,O57:O73)</f>
+        <v>200</v>
+      </c>
+      <c r="P74" s="2">
+        <f t="shared" ref="P74:Q74" si="11">SUBTOTAL(9,P57:P73)</f>
+        <v>0</v>
+      </c>
+      <c r="Q74" s="2">
+        <f t="shared" si="11"/>
+        <v>1108037</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>41</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>28</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C76" t="s">
         <v>29</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D76" t="s">
         <v>27</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G73" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="K76" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L73" s="1" t="s">
+      <c r="L76" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M73" s="1" t="s">
+      <c r="M76" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N73" s="1" t="s">
+      <c r="N76" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O73" s="1" t="s">
+      <c r="O76" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P73" s="1" t="s">
+      <c r="P76" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>1999</v>
-      </c>
-      <c r="B74">
-        <v>603800</v>
-      </c>
-      <c r="C74" t="s">
-        <v>30</v>
-      </c>
-      <c r="D74">
-        <v>4</v>
-      </c>
-      <c r="E74" t="s">
-        <v>39</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" t="s">
-        <v>11</v>
-      </c>
-      <c r="H74" s="4">
-        <v>35370</v>
-      </c>
-      <c r="I74" s="2">
-        <v>832046</v>
-      </c>
-      <c r="J74" s="2">
-        <v>832046</v>
-      </c>
-      <c r="L74" s="2">
-        <v>231619</v>
-      </c>
-      <c r="M74" s="2">
-        <v>310127</v>
-      </c>
-      <c r="N74" s="2">
-        <v>216900</v>
-      </c>
-      <c r="O74" s="2">
-        <v>73400</v>
-      </c>
-      <c r="P74" s="2">
-        <v>832046</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>1999</v>
-      </c>
-      <c r="B75">
-        <v>603800</v>
-      </c>
-      <c r="C75" t="s">
-        <v>30</v>
-      </c>
-      <c r="D75">
-        <v>4</v>
-      </c>
-      <c r="E75" t="s">
-        <v>57</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G75" t="s">
-        <v>11</v>
-      </c>
-      <c r="H75" s="4">
-        <v>35004</v>
-      </c>
-      <c r="I75" s="2">
-        <v>114000</v>
-      </c>
-      <c r="J75" s="2">
-        <v>114000</v>
-      </c>
-      <c r="K75" s="2">
-        <v>7000</v>
-      </c>
-      <c r="L75" s="2">
-        <v>25000</v>
-      </c>
-      <c r="M75" s="2">
-        <v>29000</v>
-      </c>
-      <c r="N75" s="2">
-        <v>23000</v>
-      </c>
-      <c r="O75" s="2">
-        <v>30000</v>
-      </c>
-      <c r="P75" s="2">
-        <v>114000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>1999</v>
-      </c>
-      <c r="B76">
-        <v>603800</v>
-      </c>
-      <c r="C76" t="s">
-        <v>30</v>
-      </c>
-      <c r="D76">
-        <v>4</v>
-      </c>
-      <c r="E76" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G76" t="s">
-        <v>20</v>
-      </c>
-      <c r="H76" s="4">
-        <v>34669</v>
-      </c>
-      <c r="I76" s="2">
-        <v>5448</v>
-      </c>
-      <c r="J76" s="2">
-        <v>5448</v>
-      </c>
-      <c r="K76" s="2">
-        <v>5448</v>
-      </c>
-      <c r="P76" s="2">
-        <v>5448</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -3615,28 +3636,37 @@
         <v>4</v>
       </c>
       <c r="E77" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G77" t="s">
         <v>11</v>
       </c>
       <c r="H77" s="4">
-        <v>34669</v>
+        <v>35370</v>
       </c>
       <c r="I77" s="2">
-        <v>5681</v>
+        <v>832046</v>
       </c>
       <c r="J77" s="2">
-        <v>5681</v>
-      </c>
-      <c r="K77" s="2">
-        <v>5681</v>
+        <v>832046</v>
+      </c>
+      <c r="L77" s="2">
+        <v>231619</v>
+      </c>
+      <c r="M77" s="2">
+        <v>310127</v>
+      </c>
+      <c r="N77" s="2">
+        <v>216900</v>
+      </c>
+      <c r="O77" s="2">
+        <v>73400</v>
       </c>
       <c r="P77" s="2">
-        <v>5681</v>
+        <v>832046</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -3653,10 +3683,10 @@
         <v>4</v>
       </c>
       <c r="E78" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G78" t="s">
         <v>11</v>
@@ -3665,16 +3695,28 @@
         <v>35004</v>
       </c>
       <c r="I78" s="2">
+        <v>114000</v>
+      </c>
+      <c r="J78" s="2">
+        <v>114000</v>
+      </c>
+      <c r="K78" s="2">
+        <v>7000</v>
+      </c>
+      <c r="L78" s="2">
+        <v>25000</v>
+      </c>
+      <c r="M78" s="2">
+        <v>29000</v>
+      </c>
+      <c r="N78" s="2">
+        <v>23000</v>
+      </c>
+      <c r="O78" s="2">
         <v>30000</v>
       </c>
-      <c r="J78" s="2">
-        <v>30000</v>
-      </c>
-      <c r="K78" s="2">
-        <v>30000</v>
-      </c>
       <c r="P78" s="2">
-        <v>30000</v>
+        <v>114000</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -3697,28 +3739,22 @@
         <v>21</v>
       </c>
       <c r="G79" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H79" s="4">
-        <v>35490</v>
+        <v>34669</v>
       </c>
       <c r="I79" s="2">
-        <v>29787</v>
+        <v>5448</v>
       </c>
       <c r="J79" s="2">
-        <v>29787</v>
-      </c>
-      <c r="L79" s="2">
-        <v>13859</v>
-      </c>
-      <c r="M79" s="2">
-        <v>13009</v>
-      </c>
-      <c r="N79" s="2">
-        <v>2919</v>
+        <v>5448</v>
+      </c>
+      <c r="K79" s="2">
+        <v>5448</v>
       </c>
       <c r="P79" s="2">
-        <v>29787</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -3738,28 +3774,28 @@
         <v>19</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G80" t="s">
         <v>11</v>
       </c>
       <c r="H80" s="4">
-        <v>35765</v>
+        <v>34669</v>
       </c>
       <c r="I80" s="2">
-        <v>3640</v>
+        <v>5681</v>
       </c>
       <c r="J80" s="2">
-        <v>3640</v>
-      </c>
-      <c r="L80" s="2">
-        <v>3640</v>
+        <v>5681</v>
+      </c>
+      <c r="K80" s="2">
+        <v>5681</v>
       </c>
       <c r="P80" s="2">
-        <v>3640</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5681</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1999</v>
       </c>
@@ -3776,34 +3812,28 @@
         <v>19</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G81" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H81" s="4">
-        <v>35765</v>
+        <v>35004</v>
       </c>
       <c r="I81" s="2">
-        <v>9200</v>
+        <v>30000</v>
       </c>
       <c r="J81" s="2">
-        <v>9200</v>
-      </c>
-      <c r="L81" s="2">
-        <v>2400</v>
-      </c>
-      <c r="M81" s="2">
-        <v>5600</v>
-      </c>
-      <c r="N81" s="2">
-        <v>1200</v>
+        <v>30000</v>
+      </c>
+      <c r="K81" s="2">
+        <v>30000</v>
       </c>
       <c r="P81" s="2">
-        <v>9200</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1999</v>
       </c>
@@ -3820,28 +3850,34 @@
         <v>19</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G82" t="s">
-        <v>24</v>
-      </c>
-      <c r="H82" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="H82" s="4">
+        <v>35490</v>
       </c>
       <c r="I82" s="2">
-        <v>12895</v>
+        <v>29787</v>
       </c>
       <c r="J82" s="2">
-        <v>12895</v>
-      </c>
-      <c r="K82" s="2">
-        <v>12895</v>
+        <v>29787</v>
+      </c>
+      <c r="L82" s="2">
+        <v>13859</v>
+      </c>
+      <c r="M82" s="2">
+        <v>13009</v>
+      </c>
+      <c r="N82" s="2">
+        <v>2919</v>
       </c>
       <c r="P82" s="2">
-        <v>12895</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+        <v>29787</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1999</v>
       </c>
@@ -3858,40 +3894,28 @@
         <v>19</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G83" t="s">
-        <v>26</v>
-      </c>
-      <c r="H83" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="H83" s="4">
+        <v>35765</v>
       </c>
       <c r="I83" s="2">
-        <v>21670</v>
+        <v>3640</v>
       </c>
       <c r="J83" s="2">
-        <v>21670</v>
-      </c>
-      <c r="K83" s="2">
-        <v>2214</v>
+        <v>3640</v>
       </c>
       <c r="L83" s="2">
-        <v>3706</v>
-      </c>
-      <c r="M83" s="2">
-        <v>13550</v>
-      </c>
-      <c r="N83" s="2">
-        <v>2200</v>
-      </c>
-      <c r="O83">
-        <v>0</v>
+        <v>3640</v>
       </c>
       <c r="P83" s="2">
-        <v>21670</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1999</v>
       </c>
@@ -3905,40 +3929,37 @@
         <v>4</v>
       </c>
       <c r="E84" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G84" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H84" s="4">
-        <v>35582</v>
+        <v>35765</v>
       </c>
       <c r="I84" s="2">
-        <v>10100</v>
+        <v>9200</v>
       </c>
       <c r="J84" s="2">
-        <v>10100</v>
+        <v>9200</v>
       </c>
       <c r="L84" s="2">
-        <v>3920</v>
+        <v>2400</v>
       </c>
       <c r="M84" s="2">
-        <v>6180</v>
-      </c>
-      <c r="N84">
-        <v>0</v>
-      </c>
-      <c r="O84">
-        <v>0</v>
+        <v>5600</v>
+      </c>
+      <c r="N84" s="2">
+        <v>1200</v>
       </c>
       <c r="P84" s="2">
-        <v>10100</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1999</v>
       </c>
@@ -3952,40 +3973,213 @@
         <v>4</v>
       </c>
       <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G85" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85" t="s">
+        <v>23</v>
+      </c>
+      <c r="I85" s="2">
+        <v>12895</v>
+      </c>
+      <c r="J85" s="2">
+        <v>12895</v>
+      </c>
+      <c r="K85" s="2">
+        <v>12895</v>
+      </c>
+      <c r="P85" s="2">
+        <v>12895</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1999</v>
+      </c>
+      <c r="B86">
+        <v>603800</v>
+      </c>
+      <c r="C86" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G86" t="s">
+        <v>26</v>
+      </c>
+      <c r="H86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I86" s="2">
+        <v>21670</v>
+      </c>
+      <c r="J86" s="2">
+        <v>21670</v>
+      </c>
+      <c r="K86" s="2">
+        <v>2214</v>
+      </c>
+      <c r="L86" s="2">
+        <v>3706</v>
+      </c>
+      <c r="M86" s="2">
+        <v>13550</v>
+      </c>
+      <c r="N86" s="2">
+        <v>2200</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+      <c r="P86" s="2">
+        <v>21670</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1999</v>
+      </c>
+      <c r="B87">
+        <v>603800</v>
+      </c>
+      <c r="C87" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87" t="s">
         <v>53</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="F87" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87" s="4">
+        <v>35582</v>
+      </c>
+      <c r="I87" s="2">
+        <v>10100</v>
+      </c>
+      <c r="J87" s="2">
+        <v>10100</v>
+      </c>
+      <c r="L87" s="2">
+        <v>3920</v>
+      </c>
+      <c r="M87" s="2">
+        <v>6180</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+      <c r="P87" s="2">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1999</v>
+      </c>
+      <c r="B88">
+        <v>603800</v>
+      </c>
+      <c r="C88" t="s">
+        <v>30</v>
+      </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88" t="s">
+        <v>53</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G88" t="s">
         <v>20</v>
       </c>
-      <c r="H85" s="4">
+      <c r="H88" s="4">
         <v>35855</v>
       </c>
-      <c r="I85" s="2">
+      <c r="I88" s="2">
         <v>3067</v>
       </c>
-      <c r="J85" s="2">
+      <c r="J88" s="2">
         <v>3067</v>
       </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
-      <c r="M85">
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
         <v>200</v>
       </c>
-      <c r="N85" s="2">
+      <c r="N88" s="2">
         <v>2617</v>
       </c>
-      <c r="O85">
+      <c r="O88">
         <v>250</v>
       </c>
-      <c r="P85" s="2">
+      <c r="P88" s="2">
         <v>3067</v>
       </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F89" s="3"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="2">
+        <f>SUBTOTAL(9,I72:I88)</f>
+        <v>1089134</v>
+      </c>
+      <c r="J89" s="2">
+        <f>SUBTOTAL(9,J72:J88)</f>
+        <v>1089134</v>
+      </c>
+      <c r="K89" s="2">
+        <f>SUBTOTAL(9,K72:K88)</f>
+        <v>67158</v>
+      </c>
+      <c r="L89" s="2">
+        <f t="shared" ref="L89" si="12">SUBTOTAL(9,L72:L88)</f>
+        <v>290324</v>
+      </c>
+      <c r="M89" s="2">
+        <f t="shared" ref="M89" si="13">SUBTOTAL(9,M72:M88)</f>
+        <v>379166</v>
+      </c>
+      <c r="N89" s="2">
+        <f t="shared" ref="N89" si="14">SUBTOTAL(9,N72:N88)</f>
+        <v>248836</v>
+      </c>
+      <c r="O89" s="2">
+        <f t="shared" ref="O89" si="15">SUBTOTAL(9,O72:O88)</f>
+        <v>103650</v>
+      </c>
+      <c r="P89" s="2">
+        <f t="shared" ref="P89" si="16">SUBTOTAL(9,P72:P88)</f>
+        <v>1077534</v>
+      </c>
+      <c r="Q89" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>